<commit_message>
Trace files addition and refresh scenario
</commit_message>
<xml_diff>
--- a/TESTCASES/MSD_Project_Notes_Updated.xlsx
+++ b/TESTCASES/MSD_Project_Notes_Updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MSD\PROJECT1\MSD\TESTCASES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{446F7DE7-5C9A-4E81-897E-D2AFC406C966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F90D158-0BFB-4276-81C0-B3DB21D6DC69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FCDD92B1-2F49-4B23-9115-79F9BBEC6A93}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{FCDD92B1-2F49-4B23-9115-79F9BBEC6A93}"/>
   </bookViews>
   <sheets>
     <sheet name="SPECS" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="193">
   <si>
     <t>ROW</t>
   </si>
@@ -624,6 +624,9 @@
   <si>
     <t>Accesses to different bankgroups after some 
 instructions(Adpative)</t>
+  </si>
+  <si>
+    <t>Refresh occurs when an instruction is executing</t>
   </si>
 </sst>
 </file>
@@ -1292,8 +1295,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1307,7 +1340,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1322,9 +1364,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1334,42 +1373,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1686,8 +1689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CA93103-3926-484A-A580-67BFEC347CB4}">
   <dimension ref="B1:Z28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA31" sqref="AA31"/>
+    <sheetView topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1722,14 +1725,14 @@
   <sheetData>
     <row r="1" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="E2" s="52" t="s">
+      <c r="C2" s="67"/>
+      <c r="E2" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="53"/>
+      <c r="F2" s="69"/>
       <c r="H2" s="10" t="s">
         <v>0</v>
       </c>
@@ -1804,25 +1807,25 @@
       <c r="R3" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="T3" s="68" t="s">
+      <c r="T3" s="72" t="s">
         <v>178</v>
       </c>
-      <c r="U3" s="65" t="s">
+      <c r="U3" s="70" t="s">
         <v>169</v>
       </c>
-      <c r="V3" s="54" t="s">
+      <c r="V3" s="62" t="s">
         <v>129</v>
       </c>
-      <c r="W3" s="54" t="s">
+      <c r="W3" s="62" t="s">
         <v>130</v>
       </c>
-      <c r="X3" s="54" t="s">
+      <c r="X3" s="62" t="s">
         <v>131</v>
       </c>
-      <c r="Y3" s="63" t="s">
+      <c r="Y3" s="64" t="s">
         <v>170</v>
       </c>
-      <c r="Z3" s="64"/>
+      <c r="Z3" s="65"/>
     </row>
     <row r="4" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
@@ -1849,15 +1852,15 @@
       <c r="R4" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="T4" s="71"/>
-      <c r="U4" s="72"/>
-      <c r="V4" s="49"/>
-      <c r="W4" s="49"/>
-      <c r="X4" s="49"/>
-      <c r="Y4" s="73" t="s">
+      <c r="T4" s="73"/>
+      <c r="U4" s="71"/>
+      <c r="V4" s="63"/>
+      <c r="W4" s="63"/>
+      <c r="X4" s="63"/>
+      <c r="Y4" s="52" t="s">
         <v>171</v>
       </c>
-      <c r="Z4" s="74" t="s">
+      <c r="Z4" s="53" t="s">
         <v>172</v>
       </c>
     </row>
@@ -1880,25 +1883,25 @@
       <c r="R5" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="T5" s="78" t="s">
+      <c r="T5" s="58" t="s">
         <v>184</v>
       </c>
-      <c r="U5" s="75">
-        <v>1</v>
-      </c>
-      <c r="V5" s="76">
-        <v>1</v>
-      </c>
-      <c r="W5" s="76">
-        <v>1</v>
-      </c>
-      <c r="X5" s="76">
-        <v>1</v>
-      </c>
-      <c r="Y5" s="76" t="s">
+      <c r="U5" s="54">
+        <v>1</v>
+      </c>
+      <c r="V5" s="55">
+        <v>1</v>
+      </c>
+      <c r="W5" s="55">
+        <v>1</v>
+      </c>
+      <c r="X5" s="55">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="Z5" s="77"/>
+      <c r="Z5" s="56"/>
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.25">
       <c r="E6" s="7" t="s">
@@ -1919,8 +1922,8 @@
       <c r="R6" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="T6" s="69"/>
-      <c r="U6" s="66">
+      <c r="T6" s="59"/>
+      <c r="U6" s="49">
         <v>1</v>
       </c>
       <c r="V6" s="20">
@@ -1956,8 +1959,8 @@
       <c r="R7" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="T7" s="69"/>
-      <c r="U7" s="66">
+      <c r="T7" s="59"/>
+      <c r="U7" s="49">
         <v>1</v>
       </c>
       <c r="V7" s="20">
@@ -1995,8 +1998,8 @@
       <c r="R8" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="T8" s="69"/>
-      <c r="U8" s="66">
+      <c r="T8" s="59"/>
+      <c r="U8" s="49">
         <v>1</v>
       </c>
       <c r="V8" s="20">
@@ -2034,8 +2037,8 @@
       <c r="R9" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="T9" s="59"/>
-      <c r="U9" s="67">
+      <c r="T9" s="60"/>
+      <c r="U9" s="50">
         <v>0</v>
       </c>
       <c r="V9" s="36">
@@ -2073,10 +2076,10 @@
       <c r="R10" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="T10" s="79" t="s">
+      <c r="T10" s="61" t="s">
         <v>185</v>
       </c>
-      <c r="U10" s="70">
+      <c r="U10" s="51">
         <v>1</v>
       </c>
       <c r="V10" s="44">
@@ -2112,8 +2115,8 @@
       <c r="R11" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="T11" s="69"/>
-      <c r="U11" s="66">
+      <c r="T11" s="59"/>
+      <c r="U11" s="49">
         <v>1</v>
       </c>
       <c r="V11" s="20">
@@ -2149,8 +2152,8 @@
       <c r="R12" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="T12" s="69"/>
-      <c r="U12" s="66">
+      <c r="T12" s="59"/>
+      <c r="U12" s="49">
         <v>1</v>
       </c>
       <c r="V12" s="20">
@@ -2182,8 +2185,8 @@
       <c r="R13" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="T13" s="69"/>
-      <c r="U13" s="66">
+      <c r="T13" s="59"/>
+      <c r="U13" s="49">
         <v>1</v>
       </c>
       <c r="V13" s="20">
@@ -2215,8 +2218,8 @@
       <c r="R14" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="T14" s="59"/>
-      <c r="U14" s="67">
+      <c r="T14" s="60"/>
+      <c r="U14" s="50">
         <v>0</v>
       </c>
       <c r="V14" s="36">
@@ -2248,25 +2251,25 @@
       <c r="R15" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="T15" s="78" t="s">
+      <c r="T15" s="58" t="s">
         <v>186</v>
       </c>
-      <c r="U15" s="75">
-        <v>1</v>
-      </c>
-      <c r="V15" s="76">
-        <v>1</v>
-      </c>
-      <c r="W15" s="76">
-        <v>1</v>
-      </c>
-      <c r="X15" s="76">
-        <v>1</v>
-      </c>
-      <c r="Y15" s="76" t="s">
+      <c r="U15" s="54">
+        <v>1</v>
+      </c>
+      <c r="V15" s="55">
+        <v>1</v>
+      </c>
+      <c r="W15" s="55">
+        <v>1</v>
+      </c>
+      <c r="X15" s="55">
+        <v>1</v>
+      </c>
+      <c r="Y15" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="Z15" s="77"/>
+      <c r="Z15" s="56"/>
     </row>
     <row r="16" spans="2:26" x14ac:dyDescent="0.25">
       <c r="O16" s="18" t="s">
@@ -2281,8 +2284,8 @@
       <c r="R16" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="T16" s="69"/>
-      <c r="U16" s="66">
+      <c r="T16" s="59"/>
+      <c r="U16" s="49">
         <v>1</v>
       </c>
       <c r="V16" s="20">
@@ -2312,8 +2315,8 @@
       <c r="R17" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="T17" s="69"/>
-      <c r="U17" s="66">
+      <c r="T17" s="59"/>
+      <c r="U17" s="49">
         <v>1</v>
       </c>
       <c r="V17" s="20">
@@ -2345,8 +2348,8 @@
       <c r="R18" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="T18" s="69"/>
-      <c r="U18" s="66">
+      <c r="T18" s="59"/>
+      <c r="U18" s="49">
         <v>1</v>
       </c>
       <c r="V18" s="20">
@@ -2378,8 +2381,8 @@
       <c r="R19" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="T19" s="59"/>
-      <c r="U19" s="67">
+      <c r="T19" s="60"/>
+      <c r="U19" s="50">
         <v>0</v>
       </c>
       <c r="V19" s="36">
@@ -2399,29 +2402,29 @@
       </c>
     </row>
     <row r="20" spans="15:26" x14ac:dyDescent="0.25">
-      <c r="T20" s="78" t="s">
+      <c r="T20" s="58" t="s">
         <v>187</v>
       </c>
-      <c r="U20" s="75">
-        <v>1</v>
-      </c>
-      <c r="V20" s="76">
-        <v>1</v>
-      </c>
-      <c r="W20" s="76">
-        <v>1</v>
-      </c>
-      <c r="X20" s="76">
-        <v>1</v>
-      </c>
-      <c r="Y20" s="76" t="s">
+      <c r="U20" s="54">
+        <v>1</v>
+      </c>
+      <c r="V20" s="55">
+        <v>1</v>
+      </c>
+      <c r="W20" s="55">
+        <v>1</v>
+      </c>
+      <c r="X20" s="55">
+        <v>1</v>
+      </c>
+      <c r="Y20" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="Z20" s="77"/>
+      <c r="Z20" s="56"/>
     </row>
     <row r="21" spans="15:26" x14ac:dyDescent="0.25">
-      <c r="T21" s="69"/>
-      <c r="U21" s="66">
+      <c r="T21" s="59"/>
+      <c r="U21" s="49">
         <v>1</v>
       </c>
       <c r="V21" s="20">
@@ -2439,8 +2442,8 @@
       <c r="Z21" s="22"/>
     </row>
     <row r="22" spans="15:26" x14ac:dyDescent="0.25">
-      <c r="T22" s="69"/>
-      <c r="U22" s="66">
+      <c r="T22" s="59"/>
+      <c r="U22" s="49">
         <v>1</v>
       </c>
       <c r="V22" s="20">
@@ -2460,8 +2463,8 @@
       </c>
     </row>
     <row r="23" spans="15:26" x14ac:dyDescent="0.25">
-      <c r="T23" s="69"/>
-      <c r="U23" s="66">
+      <c r="T23" s="59"/>
+      <c r="U23" s="49">
         <v>1</v>
       </c>
       <c r="V23" s="20">
@@ -2481,8 +2484,8 @@
       </c>
     </row>
     <row r="24" spans="15:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="T24" s="59"/>
-      <c r="U24" s="67">
+      <c r="T24" s="60"/>
+      <c r="U24" s="50">
         <v>0</v>
       </c>
       <c r="V24" s="36">
@@ -2502,22 +2505,17 @@
       </c>
     </row>
     <row r="27" spans="15:26" x14ac:dyDescent="0.25">
-      <c r="Y27" s="80" t="s">
+      <c r="Y27" s="57" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="28" spans="15:26" x14ac:dyDescent="0.25">
-      <c r="Y28" s="80" t="s">
+      <c r="Y28" s="57" t="s">
         <v>174</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="T5:T9"/>
-    <mergeCell ref="T15:T19"/>
-    <mergeCell ref="T10:T14"/>
-    <mergeCell ref="T20:T24"/>
-    <mergeCell ref="X3:X4"/>
     <mergeCell ref="Y3:Z3"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="E2:F2"/>
@@ -2525,6 +2523,11 @@
     <mergeCell ref="V3:V4"/>
     <mergeCell ref="W3:W4"/>
     <mergeCell ref="T3:T4"/>
+    <mergeCell ref="T5:T9"/>
+    <mergeCell ref="T15:T19"/>
+    <mergeCell ref="T10:T14"/>
+    <mergeCell ref="T20:T24"/>
+    <mergeCell ref="X3:X4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2576,8 +2579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00540E82-C942-4C51-B076-78D9BC70138E}">
   <dimension ref="B1:AP33"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="E16" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2599,7 +2602,7 @@
     <col min="17" max="17" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="11.140625" bestFit="1" customWidth="1"/>
@@ -2607,7 +2610,7 @@
     <col min="25" max="25" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="10.85546875" bestFit="1" customWidth="1"/>
@@ -2632,61 +2635,61 @@
       <c r="C2" t="s">
         <v>92</v>
       </c>
-      <c r="E2" s="56" t="s">
+      <c r="E2" s="75" t="s">
         <v>102</v>
       </c>
-      <c r="F2" s="58" t="s">
+      <c r="F2" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="60">
-        <v>1</v>
-      </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="61"/>
-      <c r="L2" s="61"/>
-      <c r="M2" s="61"/>
-      <c r="N2" s="62"/>
-      <c r="O2" s="60">
+      <c r="G2" s="78">
+        <v>1</v>
+      </c>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+      <c r="L2" s="79"/>
+      <c r="M2" s="79"/>
+      <c r="N2" s="80"/>
+      <c r="O2" s="78">
         <v>2</v>
       </c>
-      <c r="P2" s="61"/>
-      <c r="Q2" s="61"/>
-      <c r="R2" s="61"/>
-      <c r="S2" s="61"/>
-      <c r="T2" s="61"/>
-      <c r="U2" s="61"/>
-      <c r="V2" s="62"/>
-      <c r="W2" s="60">
+      <c r="P2" s="79"/>
+      <c r="Q2" s="79"/>
+      <c r="R2" s="79"/>
+      <c r="S2" s="79"/>
+      <c r="T2" s="79"/>
+      <c r="U2" s="79"/>
+      <c r="V2" s="80"/>
+      <c r="W2" s="78">
         <v>3</v>
       </c>
-      <c r="X2" s="61"/>
-      <c r="Y2" s="61"/>
-      <c r="Z2" s="61"/>
-      <c r="AA2" s="61"/>
-      <c r="AB2" s="61"/>
-      <c r="AC2" s="61"/>
-      <c r="AD2" s="62"/>
-      <c r="AE2" s="55"/>
-      <c r="AF2" s="55"/>
-      <c r="AG2" s="55"/>
-      <c r="AH2" s="55"/>
-      <c r="AI2" s="55"/>
-      <c r="AJ2" s="55"/>
-      <c r="AK2" s="55"/>
-      <c r="AL2" s="55"/>
-      <c r="AM2" s="55"/>
-      <c r="AN2" s="55"/>
-      <c r="AO2" s="55"/>
-      <c r="AP2" s="55"/>
+      <c r="X2" s="79"/>
+      <c r="Y2" s="79"/>
+      <c r="Z2" s="79"/>
+      <c r="AA2" s="79"/>
+      <c r="AB2" s="79"/>
+      <c r="AC2" s="79"/>
+      <c r="AD2" s="80"/>
+      <c r="AE2" s="74"/>
+      <c r="AF2" s="74"/>
+      <c r="AG2" s="74"/>
+      <c r="AH2" s="74"/>
+      <c r="AI2" s="74"/>
+      <c r="AJ2" s="74"/>
+      <c r="AK2" s="74"/>
+      <c r="AL2" s="74"/>
+      <c r="AM2" s="74"/>
+      <c r="AN2" s="74"/>
+      <c r="AO2" s="74"/>
+      <c r="AP2" s="74"/>
     </row>
     <row r="3" spans="2:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>93</v>
       </c>
-      <c r="E3" s="57"/>
-      <c r="F3" s="59"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="60"/>
       <c r="G3" s="30" t="s">
         <v>128</v>
       </c>
@@ -4663,29 +4666,67 @@
       <c r="E31" s="40" t="s">
         <v>164</v>
       </c>
-      <c r="F31" s="34"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
-      <c r="L31" s="20"/>
+      <c r="F31" s="34" t="s">
+        <v>192</v>
+      </c>
+      <c r="G31" s="21">
+        <v>0</v>
+      </c>
+      <c r="H31" s="19">
+        <v>1</v>
+      </c>
+      <c r="I31" s="19">
+        <v>100</v>
+      </c>
+      <c r="J31" s="19">
+        <v>128</v>
+      </c>
+      <c r="K31" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="L31" s="20">
+        <v>10</v>
+      </c>
       <c r="M31" s="47"/>
       <c r="N31" s="22"/>
-      <c r="O31" s="23"/>
-      <c r="P31" s="19"/>
-      <c r="Q31" s="19"/>
-      <c r="R31" s="19"/>
-      <c r="S31" s="19"/>
-      <c r="T31" s="20"/>
+      <c r="O31" s="23">
+        <v>0</v>
+      </c>
+      <c r="P31" s="19">
+        <v>2</v>
+      </c>
+      <c r="Q31" s="19">
+        <v>100</v>
+      </c>
+      <c r="R31" s="19">
+        <v>128</v>
+      </c>
+      <c r="S31" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="T31" s="20">
+        <v>24950</v>
+      </c>
       <c r="U31" s="47"/>
       <c r="V31" s="22"/>
-      <c r="W31" s="21"/>
-      <c r="X31" s="19"/>
-      <c r="Y31" s="19"/>
-      <c r="Z31" s="19"/>
-      <c r="AA31" s="19"/>
-      <c r="AB31" s="20"/>
+      <c r="W31" s="21">
+        <v>1</v>
+      </c>
+      <c r="X31" s="19">
+        <v>1</v>
+      </c>
+      <c r="Y31" s="19">
+        <v>100</v>
+      </c>
+      <c r="Z31" s="19">
+        <v>255</v>
+      </c>
+      <c r="AA31" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="AB31" s="20">
+        <v>25000</v>
+      </c>
       <c r="AC31" s="47"/>
       <c r="AD31" s="22"/>
     </row>

</xml_diff>